<commit_message>
Update package.db, all-profiles.xlsx, observations-summary.xlsx, StructureDefinition-my-patient.xlsx, StructureDefinition-my-patient.json, StructureDefinition-my-patient.xml, ImplementationGuide-cs6440.json, onGenerate-ig-updated.xml, qa.json, ImplementationGuide-cs6440.xml, StructureDefinition-my-patient-header.html, StructureDefinition-my-patient-sd-xref.xhtml, StructureDefinition-my-patient.ttl, StructureDefinition-my-patient-header.xhtml, StructureDefinition-weight-observation.json
</commit_message>
<xml_diff>
--- a/temp/pages/all-profiles.xlsx
+++ b/temp/pages/all-profiles.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-08T13:21:42+01:00</t>
+    <t>2024-03-08T13:24:34+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1501,7 +1501,7 @@
     <t>Observation.subject</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://example.org//StructureDefinition/my-patient)
+    <t xml:space="preserve">Reference(Patient|Group|Device|Location)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Update package.db, all-profiles.xlsx, observations-summary.xlsx, StructureDefinition-my-patient.xlsx, StructureDefinition-my-patient.json, StructureDefinition-my-patient.xml, qa.json, ImplementationGuide-cs6440.json, onGenerate-ig-updated.xml, onGenerate-ig-working.2.xml, ImplementationGuide-cs6440.xml, StructureDefinition-specific-vaccination.json, StructureDefinition-my-patient-header.html, StructureDefinition-my-patient.ttl, StructureDefinition-my-patient-header.xhtml, and ImplementationGuide-cs6440.ttl
</commit_message>
<xml_diff>
--- a/temp/pages/all-profiles.xlsx
+++ b/temp/pages/all-profiles.xlsx
@@ -63,7 +63,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-08T14:42:37+01:00</t>
+    <t>2024-03-08T14:46:34+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1504,7 +1504,7 @@
   &lt;coding&gt;
     &lt;system value="http://snomed.info/sct"/&gt;
     &lt;code value="840539006"/&gt;
-    &lt;display value="COVID-19 vaccine"/&gt;
+    &lt;display value="COVID-19"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>

</xml_diff>